<commit_message>
openpy date chart 추가
</commit_message>
<xml_diff>
--- a/python/excel_export/excel-test.xlsx
+++ b/python/excel_export/excel-test.xlsx
@@ -130,7 +130,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>Data!B2</f>
+              <f>Data!B1</f>
             </strRef>
           </tx>
           <spPr>
@@ -149,9 +149,14 @@
               </a:ln>
             </spPr>
           </marker>
+          <cat>
+            <numRef>
+              <f>Data!$A$2:$A$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>Data!$B$3:$B$8</f>
+              <f>Data!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -160,7 +165,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>Data!C2</f>
+              <f>Data!C1</f>
             </strRef>
           </tx>
           <spPr>
@@ -179,17 +184,22 @@
               </a:ln>
             </spPr>
           </marker>
+          <cat>
+            <numRef>
+              <f>Data!$A$2:$A$8</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
-              <f>Data!$C$3:$C$8</f>
+              <f>Data!$C$2:$C$8</f>
             </numRef>
           </val>
         </ser>
-        <axId val="10"/>
+        <axId val="500"/>
         <axId val="100"/>
       </lineChart>
-      <catAx>
-        <axId val="10"/>
+      <dateAx>
+        <axId val="500"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -206,11 +216,12 @@
             </rich>
           </tx>
         </title>
+        <numFmt formatCode="YY-mm-dd" sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
+        <majorTimeUnit val="days"/>
+      </dateAx>
       <valAx>
         <axId val="100"/>
         <scaling>
@@ -232,7 +243,7 @@
         </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <crossAx val="10"/>
+        <crossAx val="500"/>
       </valAx>
     </plotArea>
     <legend>
@@ -620,6 +631,9 @@
       <c r="B2" t="n">
         <v>40</v>
       </c>
+      <c r="C2" t="n">
+        <v/>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="n">
@@ -628,6 +642,9 @@
       <c r="B3" t="n">
         <v>40</v>
       </c>
+      <c r="C3" t="n">
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="n">
@@ -636,6 +653,9 @@
       <c r="B4" t="n">
         <v>50</v>
       </c>
+      <c r="C4" t="n">
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="n">
@@ -644,6 +664,9 @@
       <c r="B5" t="n">
         <v>30</v>
       </c>
+      <c r="C5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="n">
@@ -659,6 +682,9 @@
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="n">
         <v>42253</v>
+      </c>
+      <c r="B7" t="n">
+        <v/>
       </c>
       <c r="C7" t="n">
         <v>40</v>

</xml_diff>